<commit_message>
various changes to update to the fact that each script no longer needs to adjust tmin, tmax and pr to more useful units than the default.
</commit_message>
<xml_diff>
--- a/data-raw/crops/Crop_temperature_table_summary_29042020.xlsx
+++ b/data-raw/crops/Crop_temperature_table_summary_29042020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/ISIMIPData/data-raw/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BED3CE3D-1346-604C-AF8A-F93849DCCFE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B85C49-EB64-2B45-A78F-6E5756547C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49300" yWindow="4300" windowWidth="21560" windowHeight="18600" xr2:uid="{B4D76984-901C-4101-9D8A-9C2466AD7510}"/>
+    <workbookView xWindow="40980" yWindow="4300" windowWidth="29880" windowHeight="18600" xr2:uid="{B4D76984-901C-4101-9D8A-9C2466AD7510}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>Yam (African yams)</t>
   </si>
   <si>
-    <t>Tbase(℃)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Black </t>
   </si>
   <si>
@@ -303,7 +300,10 @@
     <t>Revised based on the new literature search</t>
   </si>
   <si>
-    <t>Tbase_max (℃)</t>
+    <t>Tbase</t>
+  </si>
+  <si>
+    <t>Tbase_max</t>
   </si>
 </sst>
 </file>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9915093D-623D-466F-AD80-929A98EAD566}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1003,7 +1003,7 @@
         <v>78</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="R1" s="67" t="s">
         <v>89</v>
@@ -1636,7 +1636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:20">
       <c r="A17" s="2" t="s">
         <v>71</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:20">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:20">
       <c r="A19" s="2" t="s">
         <v>69</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:20">
       <c r="A20" s="2" t="s">
         <v>69</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:20">
       <c r="A21" s="2" t="s">
         <v>71</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:20">
       <c r="A22" s="2" t="s">
         <v>74</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:20">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:20">
       <c r="A24" s="2" t="s">
         <v>73</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:20">
       <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
@@ -2041,7 +2041,7 @@
       <c r="Q25" s="48"/>
       <c r="R25" s="48"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:20">
       <c r="A26" s="2" t="s">
         <v>69</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:20">
       <c r="A27" s="2" t="s">
         <v>73</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:20">
       <c r="A28" s="1"/>
       <c r="B28" s="40"/>
       <c r="C28" s="41"/>
@@ -2154,7 +2154,7 @@
       <c r="N28" s="40"/>
       <c r="O28" s="27"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:20">
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
@@ -2169,19 +2169,19 @@
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
       <c r="O29" s="27"/>
-      <c r="Q29" s="4" t="s">
+      <c r="S29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="T29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="R29" s="4" t="s">
+    </row>
+    <row r="30" spans="1:20">
+      <c r="S30" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="Q30" s="4" t="s">
+      <c r="T30" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="R30" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>